<commit_message>
assimilate item pool names
</commit_message>
<xml_diff>
--- a/inst/extdata/items.xlsx
+++ b/inst/extdata/items.xlsx
@@ -14,13 +14,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
-    <t xml:space="preserve">Item_ID</t>
+    <t xml:space="preserve">item</t>
   </si>
   <si>
     <t xml:space="preserve">exclusions</t>
   </si>
   <si>
-    <t xml:space="preserve">RT_in_min</t>
+    <t xml:space="preserve">time</t>
   </si>
   <si>
     <t xml:space="preserve">subitems</t>
@@ -695,7 +695,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>